<commit_message>
Updated February 8, 2021
</commit_message>
<xml_diff>
--- a/wrangle/data/interventions/CIHI_closures_openings.xlsx
+++ b/wrangle/data/interventions/CIHI_closures_openings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/work/STATCAN/Projects/nick/CovidTimeline/wrangle/data/interventions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57737BC-FEC1-5A4A-9D68-2AB6CF54C958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E32DFBC-1AEB-864F-87EA-A6FA64CA01F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{B4121951-06CD-2247-ACCE-15AA6F239984}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">orig!$A$1:$L$539</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'top30'!$A$1:$M$304</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'top30'!$A$1:$M$305</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8265" uniqueCount="1882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8280" uniqueCount="1886">
   <si>
     <t>Entry ID</t>
   </si>
@@ -34097,21 +34097,6 @@
     <t>https://www.alberta.ca/release.cfm?xID=7716822CAEF42-F51A-C15A-8DA6AA1F5614D257</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">What: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Only one-on-one training is permitted for indoor fitness activities (e.g. fitness in dance studios, training figure skating on ice, one-on-one lessons). Restaurants, cafes and pubs must collect the contact information of one person from the dining party. In-person dining must close by 11 p.m. </t>
-    </r>
-  </si>
-  <si>
     <t>BC209</t>
   </si>
   <si>
@@ -34169,6 +34154,33 @@
   <si>
     <t>As of January 9, 2021, to comply with the 8 p.m. curfew, all commercial enterprises must close their doors not later than 7:30 p.m. Dining rooms are closed, Bars, brasseries, taverns, and casinos
 Closed, Personal and beauty care services closed. Effective Until: February 9, 2021.</t>
+  </si>
+  <si>
+    <t>Six rural regions in the province will be allowed to push the curfew back to 9:30 p.m. and re-open restaurants, gyms, movie theatres and some indoor activities with strict public health rules in place</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/montreal/public-health-restrictions-partial-lifting-quebec-covid-1.5896725</t>
+  </si>
+  <si>
+    <t>QC381</t>
+  </si>
+  <si>
+    <t>https://www.alberta.ca/enhanced-public-health-measures.aspx#PathForward</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Only one-on-one training is permitted for indoor fitness activities (e.g. fitness in dance studios, training figure skating on ice, one-on-one lessons). Children and youth will be allowed to participate in limited school and team sport activities. Restaurants, pubs, bars, lounges and cafes can open for in-person service. Restaurants, cafes and pubs must collect the contact information of one person from the dining party. In-person dining must close by 11 p.m. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -34510,7 +34522,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -35073,6 +35085,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Body_text" xfId="4" xr:uid="{6EABE1A5-4DA1-E64F-8051-01C7E4BEAEBC}"/>
@@ -36353,7 +36366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="120" hidden="1">
+    <row r="27" spans="1:12" ht="135" hidden="1">
       <c r="A27" s="4" t="s">
         <v>99</v>
       </c>
@@ -36857,7 +36870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="236" hidden="1">
+    <row r="41" spans="1:12" ht="253" hidden="1">
       <c r="A41" s="4" t="s">
         <v>133</v>
       </c>
@@ -37253,7 +37266,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="219" hidden="1">
+    <row r="52" spans="1:12" ht="236" hidden="1">
       <c r="A52" s="4" t="s">
         <v>169</v>
       </c>
@@ -37289,7 +37302,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="236" hidden="1">
+    <row r="53" spans="1:12" ht="253" hidden="1">
       <c r="A53" s="4" t="s">
         <v>172</v>
       </c>
@@ -37433,7 +37446,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="219" hidden="1">
+    <row r="57" spans="1:12" ht="236" hidden="1">
       <c r="A57" s="4" t="s">
         <v>183</v>
       </c>
@@ -38225,7 +38238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="253" hidden="1">
+    <row r="79" spans="1:12" ht="270" hidden="1">
       <c r="A79" s="4" t="s">
         <v>255</v>
       </c>
@@ -38693,7 +38706,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="185" hidden="1">
+    <row r="92" spans="1:12" ht="202" hidden="1">
       <c r="A92" s="4" t="s">
         <v>296</v>
       </c>
@@ -38801,7 +38814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="253" hidden="1">
+    <row r="95" spans="1:12" ht="270" hidden="1">
       <c r="A95" s="4" t="s">
         <v>305</v>
       </c>
@@ -39017,7 +39030,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="287" hidden="1">
+    <row r="101" spans="1:12" ht="304" hidden="1">
       <c r="A101" s="4" t="s">
         <v>323</v>
       </c>
@@ -39197,7 +39210,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="168" hidden="1">
+    <row r="106" spans="1:12" ht="185" hidden="1">
       <c r="A106" s="4" t="s">
         <v>334</v>
       </c>
@@ -39737,7 +39750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="100" hidden="1">
+    <row r="121" spans="1:12" ht="117" hidden="1">
       <c r="A121" s="4" t="s">
         <v>373</v>
       </c>
@@ -40205,7 +40218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="168" hidden="1">
+    <row r="134" spans="1:12" ht="185" hidden="1">
       <c r="A134" s="4" t="s">
         <v>408</v>
       </c>
@@ -40421,7 +40434,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="90" hidden="1">
+    <row r="140" spans="1:12" ht="105" hidden="1">
       <c r="A140" s="4" t="s">
         <v>423</v>
       </c>
@@ -41789,7 +41802,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="168" hidden="1">
+    <row r="178" spans="1:12" ht="185" hidden="1">
       <c r="A178" s="4" t="s">
         <v>535</v>
       </c>
@@ -41897,7 +41910,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="270" hidden="1">
+    <row r="181" spans="1:12" ht="287" hidden="1">
       <c r="A181" s="4" t="s">
         <v>544</v>
       </c>
@@ -42725,7 +42738,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="100" hidden="1">
+    <row r="204" spans="1:12" ht="117" hidden="1">
       <c r="A204" s="4" t="s">
         <v>614</v>
       </c>
@@ -42905,7 +42918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="85" hidden="1">
+    <row r="209" spans="1:12" ht="102" hidden="1">
       <c r="A209" s="4" t="s">
         <v>628</v>
       </c>
@@ -43445,7 +43458,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="83" hidden="1">
+    <row r="224" spans="1:12" ht="68" hidden="1">
       <c r="A224" s="4" t="s">
         <v>670</v>
       </c>
@@ -44489,7 +44502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="225" hidden="1">
+    <row r="253" spans="1:12" ht="240" hidden="1">
       <c r="A253" s="4" t="s">
         <v>752</v>
       </c>
@@ -44561,7 +44574,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="255" hidden="1">
+    <row r="255" spans="1:12" ht="272" hidden="1">
       <c r="A255" s="4" t="s">
         <v>760</v>
       </c>
@@ -44597,7 +44610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="256" spans="1:12" ht="85" hidden="1">
+    <row r="256" spans="1:12" ht="102" hidden="1">
       <c r="A256" s="4" t="s">
         <v>764</v>
       </c>
@@ -45029,7 +45042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="134" hidden="1">
+    <row r="268" spans="1:12" ht="151" hidden="1">
       <c r="A268" s="4" t="s">
         <v>797</v>
       </c>
@@ -45137,7 +45150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="271" spans="1:12" ht="185" hidden="1">
+    <row r="271" spans="1:12" ht="202" hidden="1">
       <c r="A271" s="4" t="s">
         <v>806</v>
       </c>
@@ -45461,7 +45474,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="280" spans="1:12" ht="402" hidden="1">
+    <row r="280" spans="1:12" ht="409.6" hidden="1">
       <c r="A280" s="4" t="s">
         <v>828</v>
       </c>
@@ -45533,7 +45546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="282" spans="1:12" ht="402" hidden="1">
+    <row r="282" spans="1:12" ht="409.6" hidden="1">
       <c r="A282" s="4" t="s">
         <v>835</v>
       </c>
@@ -45569,7 +45582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="168" hidden="1">
+    <row r="283" spans="1:12" ht="185" hidden="1">
       <c r="A283" s="4" t="s">
         <v>837</v>
       </c>
@@ -45641,7 +45654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="402" hidden="1">
+    <row r="285" spans="1:12" ht="409.6" hidden="1">
       <c r="A285" s="4" t="s">
         <v>843</v>
       </c>
@@ -46325,7 +46338,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="304" spans="1:12" ht="168" hidden="1">
+    <row r="304" spans="1:12" ht="185" hidden="1">
       <c r="A304" s="4" t="s">
         <v>901</v>
       </c>
@@ -46361,7 +46374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="305" spans="1:12" ht="134" hidden="1">
+    <row r="305" spans="1:12" ht="151" hidden="1">
       <c r="A305" s="4" t="s">
         <v>903</v>
       </c>
@@ -47009,7 +47022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="323" spans="1:12" ht="85" hidden="1">
+    <row r="323" spans="1:12" ht="90" hidden="1">
       <c r="A323" s="4" t="s">
         <v>960</v>
       </c>
@@ -47405,7 +47418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="334" spans="1:12" ht="83" hidden="1">
+    <row r="334" spans="1:12" ht="90" hidden="1">
       <c r="A334" s="4" t="s">
         <v>992</v>
       </c>
@@ -47549,7 +47562,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="338" spans="1:12" ht="83" hidden="1">
+    <row r="338" spans="1:12" ht="90" hidden="1">
       <c r="A338" s="4" t="s">
         <v>1002</v>
       </c>
@@ -48377,7 +48390,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="361" spans="1:12" ht="90" hidden="1">
+    <row r="361" spans="1:12" ht="105" hidden="1">
       <c r="A361" s="30" t="s">
         <v>1068</v>
       </c>
@@ -48449,7 +48462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="363" spans="1:12" ht="134" hidden="1">
+    <row r="363" spans="1:12" ht="151" hidden="1">
       <c r="A363" s="30" t="s">
         <v>1074</v>
       </c>
@@ -48665,7 +48678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="369" spans="1:12" ht="83" hidden="1">
+    <row r="369" spans="1:12" ht="90" hidden="1">
       <c r="A369" s="30" t="s">
         <v>1092</v>
       </c>
@@ -48773,7 +48786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="372" spans="1:12" ht="134" hidden="1">
+    <row r="372" spans="1:12" ht="151" hidden="1">
       <c r="A372" s="30" t="s">
         <v>1100</v>
       </c>
@@ -48845,7 +48858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="374" spans="1:12" ht="100" hidden="1">
+    <row r="374" spans="1:12" ht="117" hidden="1">
       <c r="A374" s="30" t="s">
         <v>1106</v>
       </c>
@@ -48881,7 +48894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="375" spans="1:12" ht="134" hidden="1">
+    <row r="375" spans="1:12" ht="151" hidden="1">
       <c r="A375" s="30" t="s">
         <v>1109</v>
       </c>
@@ -49025,7 +49038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="379" spans="1:12" ht="135" hidden="1">
+    <row r="379" spans="1:12" ht="151" hidden="1">
       <c r="A379" s="30" t="s">
         <v>1121</v>
       </c>
@@ -49097,7 +49110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="381" spans="1:12" ht="386" hidden="1">
+    <row r="381" spans="1:12" ht="402" hidden="1">
       <c r="A381" s="30" t="s">
         <v>1126</v>
       </c>
@@ -49133,7 +49146,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="382" spans="1:12" ht="151" hidden="1">
+    <row r="382" spans="1:12" ht="168" hidden="1">
       <c r="A382" s="30" t="s">
         <v>1129</v>
       </c>
@@ -49205,7 +49218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="384" spans="1:12" ht="270" hidden="1">
+    <row r="384" spans="1:12" ht="304" hidden="1">
       <c r="A384" s="30" t="s">
         <v>1135</v>
       </c>
@@ -49277,7 +49290,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="386" spans="1:12" ht="236" hidden="1">
+    <row r="386" spans="1:12" ht="253" hidden="1">
       <c r="A386" s="30" t="s">
         <v>1141</v>
       </c>
@@ -49493,7 +49506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="392" spans="1:12" ht="151" hidden="1">
+    <row r="392" spans="1:12" ht="185" hidden="1">
       <c r="A392" s="30" t="s">
         <v>1158</v>
       </c>
@@ -51257,7 +51270,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="441" spans="1:12" ht="135" hidden="1">
+    <row r="441" spans="1:12" ht="150" hidden="1">
       <c r="A441" s="61" t="s">
         <v>1300</v>
       </c>
@@ -51473,7 +51486,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="447" spans="1:12" ht="90" hidden="1">
+    <row r="447" spans="1:12" ht="105" hidden="1">
       <c r="A447" s="61" t="s">
         <v>1322</v>
       </c>
@@ -52805,7 +52818,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="484" spans="1:12" ht="135" hidden="1">
+    <row r="484" spans="1:12" ht="150" hidden="1">
       <c r="A484" s="61" t="s">
         <v>1433</v>
       </c>
@@ -55365,10 +55378,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CB1EB7-EFBB-BE4C-BF33-3C1CB63F305E}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M304"/>
+  <dimension ref="A1:M305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="H277" sqref="H277"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E305" sqref="A1:M305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -66525,7 +66538,7 @@
         <v>1566</v>
       </c>
       <c r="H274" s="129" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="I274" s="129" t="s">
         <v>1852</v>
@@ -66566,7 +66579,7 @@
         <v>1566</v>
       </c>
       <c r="H275" s="129" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="I275" s="129" t="s">
         <v>1852</v>
@@ -66607,7 +66620,7 @@
         <v>1566</v>
       </c>
       <c r="H276" s="129" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="I276" s="129" t="s">
         <v>1852</v>
@@ -66648,7 +66661,7 @@
         <v>1566</v>
       </c>
       <c r="H277" s="129" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="I277" s="129" t="s">
         <v>1852</v>
@@ -67407,7 +67420,7 @@
       </c>
       <c r="G296" s="129"/>
       <c r="H296" s="129" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="I296" s="129" t="s">
         <v>1134</v>
@@ -67547,14 +67560,18 @@
       <c r="F300" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="G300" s="129"/>
+      <c r="G300" s="129" t="s">
+        <v>1591</v>
+      </c>
       <c r="H300" s="187" t="s">
-        <v>1875</v>
+        <v>1885</v>
       </c>
       <c r="I300" s="129" t="s">
         <v>1874</v>
       </c>
-      <c r="J300" s="129"/>
+      <c r="J300" s="129" t="s">
+        <v>1884</v>
+      </c>
       <c r="K300" s="129" t="s">
         <v>18</v>
       </c>
@@ -67582,14 +67599,18 @@
       <c r="F301" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="G301" s="129"/>
+      <c r="G301" s="129" t="s">
+        <v>1591</v>
+      </c>
       <c r="H301" s="187" t="s">
-        <v>1875</v>
+        <v>1885</v>
       </c>
       <c r="I301" s="129" t="s">
         <v>1874</v>
       </c>
-      <c r="J301" s="129"/>
+      <c r="J301" s="129" t="s">
+        <v>1884</v>
+      </c>
       <c r="K301" s="129" t="s">
         <v>18</v>
       </c>
@@ -67617,14 +67638,18 @@
       <c r="F302" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="G302" s="129"/>
+      <c r="G302" s="129" t="s">
+        <v>1591</v>
+      </c>
       <c r="H302" s="187" t="s">
-        <v>1875</v>
+        <v>1885</v>
       </c>
       <c r="I302" s="129" t="s">
         <v>1874</v>
       </c>
-      <c r="J302" s="129"/>
+      <c r="J302" s="129" t="s">
+        <v>1884</v>
+      </c>
       <c r="K302" s="129" t="s">
         <v>18</v>
       </c>
@@ -67637,7 +67662,7 @@
     </row>
     <row r="303" spans="1:13" hidden="1">
       <c r="A303" s="187" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B303" s="129" t="s">
         <v>143</v>
@@ -67660,7 +67685,7 @@
     </row>
     <row r="304" spans="1:13" hidden="1">
       <c r="A304" s="187" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B304" s="110" t="s">
         <v>260</v>
@@ -67679,10 +67704,10 @@
       </c>
       <c r="G304" s="129"/>
       <c r="H304" s="129" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="I304" s="129" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="J304" s="129"/>
       <c r="K304" s="129" t="s">
@@ -67695,8 +67720,45 @@
         <v>1847</v>
       </c>
     </row>
+    <row r="305" spans="1:13">
+      <c r="A305" s="212" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B305" s="106" t="s">
+        <v>950</v>
+      </c>
+      <c r="C305" s="137" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D305" s="178">
+        <v>44232</v>
+      </c>
+      <c r="E305" s="178">
+        <v>44235</v>
+      </c>
+      <c r="F305" s="179" t="s">
+        <v>59</v>
+      </c>
+      <c r="G305" s="137"/>
+      <c r="H305" s="137" t="s">
+        <v>1881</v>
+      </c>
+      <c r="I305" s="137" t="s">
+        <v>1882</v>
+      </c>
+      <c r="J305" s="137"/>
+      <c r="K305" s="106" t="s">
+        <v>91</v>
+      </c>
+      <c r="L305" s="106" t="s">
+        <v>19</v>
+      </c>
+      <c r="M305" s="189" t="s">
+        <v>1846</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M304" xr:uid="{2E928349-A5AA-9B41-9E5A-C956A9EBD262}">
+  <autoFilter ref="A1:M305" xr:uid="{2E928349-A5AA-9B41-9E5A-C956A9EBD262}">
     <filterColumn colId="1">
       <filters>
         <filter val="Que."/>

</xml_diff>

<commit_message>
Updated February 15, 2021.
</commit_message>
<xml_diff>
--- a/wrangle/data/interventions/CIHI_closures_openings.xlsx
+++ b/wrangle/data/interventions/CIHI_closures_openings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/work/STATCAN/Projects/nick/CovidTimeline/wrangle/data/interventions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E32DFBC-1AEB-864F-87EA-A6FA64CA01F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D73F34-9588-2740-8612-96FE4F07A81C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{B4121951-06CD-2247-ACCE-15AA6F239984}"/>
+    <workbookView xWindow="4020" yWindow="1100" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{B4121951-06CD-2247-ACCE-15AA6F239984}"/>
   </bookViews>
   <sheets>
     <sheet name="orig" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">orig!$A$1:$L$539</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'top30'!$A$1:$M$305</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'top30'!$A$1:$M$315</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8280" uniqueCount="1886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8382" uniqueCount="1894">
   <si>
     <t>Entry ID</t>
   </si>
@@ -34181,6 +34181,31 @@
       </rPr>
       <t xml:space="preserve">Only one-on-one training is permitted for indoor fitness activities (e.g. fitness in dance studios, training figure skating on ice, one-on-one lessons). Children and youth will be allowed to participate in limited school and team sport activities. Restaurants, pubs, bars, lounges and cafes can open for in-person service. Restaurants, cafes and pubs must collect the contact information of one person from the dining party. In-person dining must close by 11 p.m. </t>
     </r>
+  </si>
+  <si>
+    <t>ON267</t>
+  </si>
+  <si>
+    <t>https://globalnews.ca/news/7627151/ontario-coronavirus-phased-reopening-covid-19/</t>
+  </si>
+  <si>
+    <t>https://news.ontario.ca/en/backgrounder/60260/in-person-shopping-at-retail-stores-permitted-with-public-health-and-safety-requirements-in-place</t>
+  </si>
+  <si>
+    <t>In person shopping permitted for retail sales, with capacity limits;75 per cent capacity limit for supermarkets and other stores that primarily sell groceries, convenience stores, and pharmacies; and
+50 per cent capacity limit for all other retail businesses that engage in retail sales to the public, including big box stores;</t>
+  </si>
+  <si>
+    <t>ON268</t>
+  </si>
+  <si>
+    <t>https://news.ontario.ca/en/release/60339/ontario-returning-27-public-health-regions-to-strengthened-covid-19-response-framework</t>
+  </si>
+  <si>
+    <t>Level 3 (Orange)</t>
+  </si>
+  <si>
+    <t>Restaurants &amp; eating places, Activities</t>
   </si>
 </sst>
 </file>
@@ -34192,7 +34217,7 @@
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -34332,6 +34357,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -34371,7 +34403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -34509,6 +34541,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -34522,7 +34567,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -35086,6 +35131,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Body_text" xfId="4" xr:uid="{6EABE1A5-4DA1-E64F-8051-01C7E4BEAEBC}"/>
@@ -36366,7 +36421,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="135" hidden="1">
+    <row r="27" spans="1:12" ht="120" hidden="1">
       <c r="A27" s="4" t="s">
         <v>99</v>
       </c>
@@ -36870,7 +36925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="253" hidden="1">
+    <row r="41" spans="1:12" ht="236" hidden="1">
       <c r="A41" s="4" t="s">
         <v>133</v>
       </c>
@@ -37266,7 +37321,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="236" hidden="1">
+    <row r="52" spans="1:12" ht="219" hidden="1">
       <c r="A52" s="4" t="s">
         <v>169</v>
       </c>
@@ -37302,7 +37357,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="253" hidden="1">
+    <row r="53" spans="1:12" ht="236" hidden="1">
       <c r="A53" s="4" t="s">
         <v>172</v>
       </c>
@@ -37446,7 +37501,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="236" hidden="1">
+    <row r="57" spans="1:12" ht="219" hidden="1">
       <c r="A57" s="4" t="s">
         <v>183</v>
       </c>
@@ -38238,7 +38293,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="270" hidden="1">
+    <row r="79" spans="1:12" ht="253" hidden="1">
       <c r="A79" s="4" t="s">
         <v>255</v>
       </c>
@@ -38706,7 +38761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="202" hidden="1">
+    <row r="92" spans="1:12" ht="185" hidden="1">
       <c r="A92" s="4" t="s">
         <v>296</v>
       </c>
@@ -38814,7 +38869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="270" hidden="1">
+    <row r="95" spans="1:12" ht="253" hidden="1">
       <c r="A95" s="4" t="s">
         <v>305</v>
       </c>
@@ -39030,7 +39085,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="304" hidden="1">
+    <row r="101" spans="1:12" ht="287" hidden="1">
       <c r="A101" s="4" t="s">
         <v>323</v>
       </c>
@@ -39210,7 +39265,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="185" hidden="1">
+    <row r="106" spans="1:12" ht="168" hidden="1">
       <c r="A106" s="4" t="s">
         <v>334</v>
       </c>
@@ -39750,7 +39805,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="117" hidden="1">
+    <row r="121" spans="1:12" ht="100" hidden="1">
       <c r="A121" s="4" t="s">
         <v>373</v>
       </c>
@@ -40218,7 +40273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="185" hidden="1">
+    <row r="134" spans="1:12" ht="168" hidden="1">
       <c r="A134" s="4" t="s">
         <v>408</v>
       </c>
@@ -40434,7 +40489,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="105" hidden="1">
+    <row r="140" spans="1:12" ht="90" hidden="1">
       <c r="A140" s="4" t="s">
         <v>423</v>
       </c>
@@ -41802,7 +41857,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="185" hidden="1">
+    <row r="178" spans="1:12" ht="168" hidden="1">
       <c r="A178" s="4" t="s">
         <v>535</v>
       </c>
@@ -41910,7 +41965,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="287" hidden="1">
+    <row r="181" spans="1:12" ht="270" hidden="1">
       <c r="A181" s="4" t="s">
         <v>544</v>
       </c>
@@ -42738,7 +42793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="117" hidden="1">
+    <row r="204" spans="1:12" ht="100" hidden="1">
       <c r="A204" s="4" t="s">
         <v>614</v>
       </c>
@@ -42918,7 +42973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="102" hidden="1">
+    <row r="209" spans="1:12" ht="85" hidden="1">
       <c r="A209" s="4" t="s">
         <v>628</v>
       </c>
@@ -43458,7 +43513,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="68" hidden="1">
+    <row r="224" spans="1:12" ht="83" hidden="1">
       <c r="A224" s="4" t="s">
         <v>670</v>
       </c>
@@ -44502,7 +44557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="240" hidden="1">
+    <row r="253" spans="1:12" ht="225" hidden="1">
       <c r="A253" s="4" t="s">
         <v>752</v>
       </c>
@@ -44574,7 +44629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="272" hidden="1">
+    <row r="255" spans="1:12" ht="255" hidden="1">
       <c r="A255" s="4" t="s">
         <v>760</v>
       </c>
@@ -44610,7 +44665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="256" spans="1:12" ht="102" hidden="1">
+    <row r="256" spans="1:12" ht="85" hidden="1">
       <c r="A256" s="4" t="s">
         <v>764</v>
       </c>
@@ -45042,7 +45097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="151" hidden="1">
+    <row r="268" spans="1:12" ht="134" hidden="1">
       <c r="A268" s="4" t="s">
         <v>797</v>
       </c>
@@ -45150,7 +45205,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="271" spans="1:12" ht="202" hidden="1">
+    <row r="271" spans="1:12" ht="185" hidden="1">
       <c r="A271" s="4" t="s">
         <v>806</v>
       </c>
@@ -45474,7 +45529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="280" spans="1:12" ht="409.6" hidden="1">
+    <row r="280" spans="1:12" ht="402" hidden="1">
       <c r="A280" s="4" t="s">
         <v>828</v>
       </c>
@@ -45546,7 +45601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="282" spans="1:12" ht="409.6" hidden="1">
+    <row r="282" spans="1:12" ht="402" hidden="1">
       <c r="A282" s="4" t="s">
         <v>835</v>
       </c>
@@ -45582,7 +45637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="185" hidden="1">
+    <row r="283" spans="1:12" ht="168" hidden="1">
       <c r="A283" s="4" t="s">
         <v>837</v>
       </c>
@@ -45654,7 +45709,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="409.6" hidden="1">
+    <row r="285" spans="1:12" ht="402" hidden="1">
       <c r="A285" s="4" t="s">
         <v>843</v>
       </c>
@@ -46338,7 +46393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="304" spans="1:12" ht="185" hidden="1">
+    <row r="304" spans="1:12" ht="168" hidden="1">
       <c r="A304" s="4" t="s">
         <v>901</v>
       </c>
@@ -46374,7 +46429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="305" spans="1:12" ht="151" hidden="1">
+    <row r="305" spans="1:12" ht="134" hidden="1">
       <c r="A305" s="4" t="s">
         <v>903</v>
       </c>
@@ -47022,7 +47077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="323" spans="1:12" ht="90" hidden="1">
+    <row r="323" spans="1:12" ht="85" hidden="1">
       <c r="A323" s="4" t="s">
         <v>960</v>
       </c>
@@ -47418,7 +47473,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="334" spans="1:12" ht="90" hidden="1">
+    <row r="334" spans="1:12" ht="83" hidden="1">
       <c r="A334" s="4" t="s">
         <v>992</v>
       </c>
@@ -47562,7 +47617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="338" spans="1:12" ht="90" hidden="1">
+    <row r="338" spans="1:12" ht="83" hidden="1">
       <c r="A338" s="4" t="s">
         <v>1002</v>
       </c>
@@ -48390,7 +48445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="361" spans="1:12" ht="105" hidden="1">
+    <row r="361" spans="1:12" ht="90" hidden="1">
       <c r="A361" s="30" t="s">
         <v>1068</v>
       </c>
@@ -48462,7 +48517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="363" spans="1:12" ht="151" hidden="1">
+    <row r="363" spans="1:12" ht="134" hidden="1">
       <c r="A363" s="30" t="s">
         <v>1074</v>
       </c>
@@ -48678,7 +48733,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="369" spans="1:12" ht="90" hidden="1">
+    <row r="369" spans="1:12" ht="83" hidden="1">
       <c r="A369" s="30" t="s">
         <v>1092</v>
       </c>
@@ -48786,7 +48841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="372" spans="1:12" ht="151" hidden="1">
+    <row r="372" spans="1:12" ht="134" hidden="1">
       <c r="A372" s="30" t="s">
         <v>1100</v>
       </c>
@@ -48858,7 +48913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="374" spans="1:12" ht="117" hidden="1">
+    <row r="374" spans="1:12" ht="100" hidden="1">
       <c r="A374" s="30" t="s">
         <v>1106</v>
       </c>
@@ -48894,7 +48949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="375" spans="1:12" ht="151" hidden="1">
+    <row r="375" spans="1:12" ht="134" hidden="1">
       <c r="A375" s="30" t="s">
         <v>1109</v>
       </c>
@@ -49038,7 +49093,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="379" spans="1:12" ht="151" hidden="1">
+    <row r="379" spans="1:12" ht="135" hidden="1">
       <c r="A379" s="30" t="s">
         <v>1121</v>
       </c>
@@ -49110,7 +49165,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="381" spans="1:12" ht="402" hidden="1">
+    <row r="381" spans="1:12" ht="386" hidden="1">
       <c r="A381" s="30" t="s">
         <v>1126</v>
       </c>
@@ -49146,7 +49201,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="382" spans="1:12" ht="168" hidden="1">
+    <row r="382" spans="1:12" ht="151" hidden="1">
       <c r="A382" s="30" t="s">
         <v>1129</v>
       </c>
@@ -49218,7 +49273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="384" spans="1:12" ht="304" hidden="1">
+    <row r="384" spans="1:12" ht="270" hidden="1">
       <c r="A384" s="30" t="s">
         <v>1135</v>
       </c>
@@ -49290,7 +49345,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="386" spans="1:12" ht="253" hidden="1">
+    <row r="386" spans="1:12" ht="236" hidden="1">
       <c r="A386" s="30" t="s">
         <v>1141</v>
       </c>
@@ -49506,7 +49561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="392" spans="1:12" ht="185" hidden="1">
+    <row r="392" spans="1:12" ht="151" hidden="1">
       <c r="A392" s="30" t="s">
         <v>1158</v>
       </c>
@@ -51270,7 +51325,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="441" spans="1:12" ht="150" hidden="1">
+    <row r="441" spans="1:12" ht="135" hidden="1">
       <c r="A441" s="61" t="s">
         <v>1300</v>
       </c>
@@ -51486,7 +51541,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="447" spans="1:12" ht="105" hidden="1">
+    <row r="447" spans="1:12" ht="90" hidden="1">
       <c r="A447" s="61" t="s">
         <v>1322</v>
       </c>
@@ -52818,7 +52873,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="484" spans="1:12" ht="150" hidden="1">
+    <row r="484" spans="1:12" ht="135" hidden="1">
       <c r="A484" s="61" t="s">
         <v>1433</v>
       </c>
@@ -55378,10 +55433,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55CB1EB7-EFBB-BE4C-BF33-3C1CB63F305E}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:M305"/>
+  <dimension ref="A1:M315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E305" sqref="A1:M305"/>
+      <selection activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -58599,7 +58654,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1">
+    <row r="80" spans="1:13">
       <c r="A80" s="155" t="s">
         <v>1685</v>
       </c>
@@ -58640,7 +58695,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1">
+    <row r="81" spans="1:13">
       <c r="A81" s="155" t="s">
         <v>1685</v>
       </c>
@@ -58681,7 +58736,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="186" customFormat="1" hidden="1">
+    <row r="82" spans="1:13" s="186" customFormat="1">
       <c r="A82" s="155" t="s">
         <v>1689</v>
       </c>
@@ -58722,7 +58777,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="186" customFormat="1" hidden="1">
+    <row r="83" spans="1:13" s="186" customFormat="1">
       <c r="A83" s="155" t="s">
         <v>1689</v>
       </c>
@@ -58763,7 +58818,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1">
+    <row r="84" spans="1:13">
       <c r="A84" s="155" t="s">
         <v>1693</v>
       </c>
@@ -58804,7 +58859,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1">
+    <row r="85" spans="1:13">
       <c r="A85" s="155" t="s">
         <v>1693</v>
       </c>
@@ -58845,7 +58900,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="60" hidden="1">
+    <row r="86" spans="1:13" ht="60">
       <c r="A86" s="155" t="s">
         <v>1696</v>
       </c>
@@ -58886,7 +58941,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1">
+    <row r="87" spans="1:13">
       <c r="A87" s="155" t="s">
         <v>1696</v>
       </c>
@@ -58927,7 +58982,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1">
+    <row r="88" spans="1:13">
       <c r="A88" s="155" t="s">
         <v>1790</v>
       </c>
@@ -58966,7 +59021,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1">
+    <row r="89" spans="1:13">
       <c r="A89" s="155" t="s">
         <v>1803</v>
       </c>
@@ -59005,7 +59060,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1">
+    <row r="90" spans="1:13">
       <c r="A90" s="197" t="s">
         <v>1794</v>
       </c>
@@ -59044,7 +59099,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1">
+    <row r="91" spans="1:13">
       <c r="A91" s="197" t="s">
         <v>1804</v>
       </c>
@@ -63245,7 +63300,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" hidden="1">
       <c r="A194" s="177" t="s">
         <v>1569</v>
       </c>
@@ -63286,7 +63341,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" hidden="1">
       <c r="A195" s="176" t="s">
         <v>1572</v>
       </c>
@@ -63327,7 +63382,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" hidden="1">
       <c r="A196" s="180" t="s">
         <v>1576</v>
       </c>
@@ -63368,7 +63423,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" hidden="1">
       <c r="A197" s="155" t="s">
         <v>1714</v>
       </c>
@@ -63409,7 +63464,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" hidden="1">
       <c r="A198" s="155" t="s">
         <v>1714</v>
       </c>
@@ -63450,7 +63505,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" hidden="1">
       <c r="A199" s="155" t="s">
         <v>1714</v>
       </c>
@@ -63491,7 +63546,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" hidden="1">
       <c r="A200" s="155" t="s">
         <v>1714</v>
       </c>
@@ -63532,7 +63587,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" hidden="1">
       <c r="A201" s="155" t="s">
         <v>1714</v>
       </c>
@@ -63573,7 +63628,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" hidden="1">
       <c r="A202" s="155" t="s">
         <v>1718</v>
       </c>
@@ -63614,7 +63669,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" hidden="1">
       <c r="A203" s="155" t="s">
         <v>1718</v>
       </c>
@@ -63655,7 +63710,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" hidden="1">
       <c r="A204" s="155" t="s">
         <v>1718</v>
       </c>
@@ -63696,7 +63751,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" hidden="1">
       <c r="A205" s="155" t="s">
         <v>1718</v>
       </c>
@@ -63737,7 +63792,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" hidden="1">
       <c r="A206" s="155" t="s">
         <v>1718</v>
       </c>
@@ -63778,7 +63833,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" hidden="1">
       <c r="A207" s="155" t="s">
         <v>1720</v>
       </c>
@@ -63819,7 +63874,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" hidden="1">
       <c r="A208" s="155" t="s">
         <v>1720</v>
       </c>
@@ -63860,7 +63915,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" hidden="1">
       <c r="A209" s="155" t="s">
         <v>1720</v>
       </c>
@@ -63901,7 +63956,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" hidden="1">
       <c r="A210" s="155" t="s">
         <v>1720</v>
       </c>
@@ -63942,7 +63997,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" hidden="1">
       <c r="A211" s="155" t="s">
         <v>1720</v>
       </c>
@@ -63983,7 +64038,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" hidden="1">
       <c r="A212" s="155" t="s">
         <v>1758</v>
       </c>
@@ -64024,7 +64079,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" hidden="1">
       <c r="A213" s="155" t="s">
         <v>1758</v>
       </c>
@@ -64065,7 +64120,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" hidden="1">
       <c r="A214" s="155" t="s">
         <v>1758</v>
       </c>
@@ -64106,7 +64161,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" hidden="1">
       <c r="A215" s="155" t="s">
         <v>1758</v>
       </c>
@@ -64147,7 +64202,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" hidden="1">
       <c r="A216" s="155" t="s">
         <v>1758</v>
       </c>
@@ -64188,7 +64243,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" hidden="1">
       <c r="A217" s="155" t="s">
         <v>1722</v>
       </c>
@@ -64229,7 +64284,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" hidden="1">
       <c r="A218" s="155" t="s">
         <v>1722</v>
       </c>
@@ -64270,7 +64325,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" hidden="1">
       <c r="A219" s="155" t="s">
         <v>1722</v>
       </c>
@@ -64311,7 +64366,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" hidden="1">
       <c r="A220" s="155" t="s">
         <v>1722</v>
       </c>
@@ -64352,7 +64407,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" hidden="1">
       <c r="A221" s="155" t="s">
         <v>1722</v>
       </c>
@@ -64393,7 +64448,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="75">
+    <row r="222" spans="1:13" ht="75" hidden="1">
       <c r="A222" s="155" t="s">
         <v>1725</v>
       </c>
@@ -64434,7 +64489,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" hidden="1">
       <c r="A223" s="155" t="s">
         <v>1725</v>
       </c>
@@ -64475,7 +64530,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" hidden="1">
       <c r="A224" s="155" t="s">
         <v>1725</v>
       </c>
@@ -64516,7 +64571,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" hidden="1">
       <c r="A225" s="155" t="s">
         <v>1725</v>
       </c>
@@ -64557,7 +64612,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" hidden="1">
       <c r="A226" s="155" t="s">
         <v>1725</v>
       </c>
@@ -64598,7 +64653,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" hidden="1">
       <c r="A227" s="155" t="s">
         <v>1729</v>
       </c>
@@ -64639,7 +64694,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" hidden="1">
       <c r="A228" s="155" t="s">
         <v>1729</v>
       </c>
@@ -64680,7 +64735,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" hidden="1">
       <c r="A229" s="155" t="s">
         <v>1760</v>
       </c>
@@ -64721,7 +64776,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" hidden="1">
       <c r="A230" s="155" t="s">
         <v>1760</v>
       </c>
@@ -64762,7 +64817,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" hidden="1">
       <c r="A231" s="155" t="s">
         <v>1760</v>
       </c>
@@ -64803,7 +64858,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" hidden="1">
       <c r="A232" s="155" t="s">
         <v>1760</v>
       </c>
@@ -64844,7 +64899,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" hidden="1">
       <c r="A233" s="155" t="s">
         <v>1760</v>
       </c>
@@ -64885,7 +64940,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" hidden="1">
       <c r="A234" s="155" t="s">
         <v>1732</v>
       </c>
@@ -64926,7 +64981,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" hidden="1">
       <c r="A235" s="155" t="s">
         <v>1732</v>
       </c>
@@ -64967,7 +65022,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" hidden="1">
       <c r="A236" s="155" t="s">
         <v>1732</v>
       </c>
@@ -65008,7 +65063,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" hidden="1">
       <c r="A237" s="155" t="s">
         <v>1732</v>
       </c>
@@ -65049,7 +65104,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" hidden="1">
       <c r="A238" s="155" t="s">
         <v>1732</v>
       </c>
@@ -65090,7 +65145,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" hidden="1">
       <c r="A239" s="155" t="s">
         <v>1736</v>
       </c>
@@ -65131,7 +65186,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" hidden="1">
       <c r="A240" s="155" t="s">
         <v>1736</v>
       </c>
@@ -65172,7 +65227,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" hidden="1">
       <c r="A241" s="155" t="s">
         <v>1736</v>
       </c>
@@ -65213,7 +65268,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" hidden="1">
       <c r="A242" s="155" t="s">
         <v>1736</v>
       </c>
@@ -65254,7 +65309,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" hidden="1">
       <c r="A243" s="155" t="s">
         <v>1736</v>
       </c>
@@ -65295,7 +65350,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" hidden="1">
       <c r="A244" s="155" t="s">
         <v>1739</v>
       </c>
@@ -65336,7 +65391,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" hidden="1">
       <c r="A245" s="155" t="s">
         <v>1739</v>
       </c>
@@ -65377,7 +65432,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" hidden="1">
       <c r="A246" s="155" t="s">
         <v>1739</v>
       </c>
@@ -65418,7 +65473,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" hidden="1">
       <c r="A247" s="155" t="s">
         <v>1739</v>
       </c>
@@ -65459,7 +65514,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" hidden="1">
       <c r="A248" s="155" t="s">
         <v>1739</v>
       </c>
@@ -65500,7 +65555,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" hidden="1">
       <c r="A249" s="155" t="s">
         <v>1742</v>
       </c>
@@ -65541,7 +65596,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" hidden="1">
       <c r="A250" s="155" t="s">
         <v>1742</v>
       </c>
@@ -65582,7 +65637,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" hidden="1">
       <c r="A251" s="155" t="s">
         <v>1742</v>
       </c>
@@ -65623,7 +65678,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" hidden="1">
       <c r="A252" s="155" t="s">
         <v>1742</v>
       </c>
@@ -65664,7 +65719,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" hidden="1">
       <c r="A253" s="155" t="s">
         <v>1742</v>
       </c>
@@ -65705,7 +65760,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" hidden="1">
       <c r="A254" s="114" t="s">
         <v>1767</v>
       </c>
@@ -65746,7 +65801,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" hidden="1">
       <c r="A255" s="114" t="s">
         <v>1810</v>
       </c>
@@ -65787,7 +65842,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" hidden="1">
       <c r="A256" s="114" t="s">
         <v>1813</v>
       </c>
@@ -65828,7 +65883,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" hidden="1">
       <c r="A257" s="114" t="s">
         <v>1813</v>
       </c>
@@ -65867,7 +65922,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" hidden="1">
       <c r="A258" s="187" t="s">
         <v>1814</v>
       </c>
@@ -65906,7 +65961,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" hidden="1">
       <c r="A259" s="187" t="s">
         <v>1814</v>
       </c>
@@ -65945,7 +66000,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" hidden="1">
       <c r="A260" s="187" t="s">
         <v>1814</v>
       </c>
@@ -65984,7 +66039,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" hidden="1">
       <c r="A261" s="187" t="s">
         <v>1814</v>
       </c>
@@ -66515,7 +66570,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" hidden="1">
       <c r="A274" s="187" t="s">
         <v>1843</v>
       </c>
@@ -66556,7 +66611,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" hidden="1">
       <c r="A275" s="187" t="s">
         <v>1843</v>
       </c>
@@ -66597,7 +66652,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" hidden="1">
       <c r="A276" s="187" t="s">
         <v>1843</v>
       </c>
@@ -66638,7 +66693,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" hidden="1">
       <c r="A277" s="187" t="s">
         <v>1843</v>
       </c>
@@ -66699,7 +66754,7 @@
         <v>1780</v>
       </c>
       <c r="G278" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H278" s="129" t="s">
         <v>1850</v>
@@ -66740,7 +66795,7 @@
         <v>1780</v>
       </c>
       <c r="G279" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H279" s="129" t="s">
         <v>1850</v>
@@ -66781,7 +66836,7 @@
         <v>1780</v>
       </c>
       <c r="G280" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H280" s="129" t="s">
         <v>1850</v>
@@ -66822,7 +66877,7 @@
         <v>1780</v>
       </c>
       <c r="G281" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H281" s="129" t="s">
         <v>1850</v>
@@ -66863,7 +66918,7 @@
         <v>1780</v>
       </c>
       <c r="G282" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H282" s="129" t="s">
         <v>1850</v>
@@ -66904,7 +66959,7 @@
         <v>1780</v>
       </c>
       <c r="G283" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H283" s="129" t="s">
         <v>1850</v>
@@ -66945,7 +67000,7 @@
         <v>1780</v>
       </c>
       <c r="G284" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H284" s="129" t="s">
         <v>1850</v>
@@ -66986,7 +67041,7 @@
         <v>1780</v>
       </c>
       <c r="G285" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H285" s="129" t="s">
         <v>1850</v>
@@ -67027,7 +67082,7 @@
         <v>1780</v>
       </c>
       <c r="G286" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H286" s="129" t="s">
         <v>1850</v>
@@ -67068,7 +67123,7 @@
         <v>1780</v>
       </c>
       <c r="G287" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H287" s="129" t="s">
         <v>1850</v>
@@ -67109,7 +67164,7 @@
         <v>1780</v>
       </c>
       <c r="G288" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H288" s="129" t="s">
         <v>1850</v>
@@ -67150,7 +67205,7 @@
         <v>1780</v>
       </c>
       <c r="G289" s="115" t="s">
-        <v>1566</v>
+        <v>1608</v>
       </c>
       <c r="H289" s="129" t="s">
         <v>1850</v>
@@ -67204,7 +67259,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="291" spans="1:13" hidden="1">
+    <row r="291" spans="1:13">
       <c r="A291" s="187" t="s">
         <v>1860</v>
       </c>
@@ -67245,7 +67300,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="292" spans="1:13" hidden="1">
+    <row r="292" spans="1:13">
       <c r="A292" s="187" t="s">
         <v>1860</v>
       </c>
@@ -67720,7 +67775,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" hidden="1">
       <c r="A305" s="212" t="s">
         <v>1883</v>
       </c>
@@ -67739,7 +67794,9 @@
       <c r="F305" s="179" t="s">
         <v>59</v>
       </c>
-      <c r="G305" s="137"/>
+      <c r="G305" s="137" t="s">
+        <v>1892</v>
+      </c>
       <c r="H305" s="137" t="s">
         <v>1881</v>
       </c>
@@ -67757,11 +67814,394 @@
         <v>1846</v>
       </c>
     </row>
+    <row r="306" spans="1:13" ht="85" hidden="1">
+      <c r="A306" s="188" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B306" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C306" s="206" t="s">
+        <v>1771</v>
+      </c>
+      <c r="D306" s="213">
+        <v>44235</v>
+      </c>
+      <c r="E306" s="213">
+        <v>44237</v>
+      </c>
+      <c r="F306" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G306" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H306" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I306" s="154" t="s">
+        <v>1887</v>
+      </c>
+      <c r="J306" s="154" t="s">
+        <v>1888</v>
+      </c>
+      <c r="K306" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L306" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M306" s="189" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" ht="85" hidden="1">
+      <c r="A307" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B307" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C307" s="206" t="s">
+        <v>1532</v>
+      </c>
+      <c r="D307" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E307" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F307" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G307" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H307" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I307" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K307" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L307" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M307" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" ht="85" hidden="1">
+      <c r="A308" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B308" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C308" s="206" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D308" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E308" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F308" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G308" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H308" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I308" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K308" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L308" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M308" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" ht="85" hidden="1">
+      <c r="A309" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B309" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C309" s="206" t="s">
+        <v>1515</v>
+      </c>
+      <c r="D309" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E309" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F309" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G309" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H309" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I309" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K309" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L309" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M309" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" ht="85" hidden="1">
+      <c r="A310" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B310" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C310" s="206" t="s">
+        <v>1536</v>
+      </c>
+      <c r="D310" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E310" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F310" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G310" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H310" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I310" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K310" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L310" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M310" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" ht="85" hidden="1">
+      <c r="A311" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B311" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C311" s="206" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D311" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E311" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F311" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G311" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H311" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I311" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K311" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L311" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M311" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" ht="85" hidden="1">
+      <c r="A312" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B312" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C312" s="206" t="s">
+        <v>1542</v>
+      </c>
+      <c r="D312" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E312" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F312" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G312" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H312" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I312" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K312" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L312" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M312" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" ht="85" hidden="1">
+      <c r="A313" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B313" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C313" s="206" t="s">
+        <v>1529</v>
+      </c>
+      <c r="D313" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E313" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F313" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G313" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H313" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I313" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K313" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L313" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M313" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" ht="85" hidden="1">
+      <c r="A314" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B314" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C314" s="206" t="s">
+        <v>1530</v>
+      </c>
+      <c r="D314" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E314" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F314" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G314" s="214" t="s">
+        <v>1566</v>
+      </c>
+      <c r="H314" s="215" t="s">
+        <v>1889</v>
+      </c>
+      <c r="I314" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K314" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L314" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M314" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" hidden="1">
+      <c r="A315" s="188" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B315" s="206" t="s">
+        <v>712</v>
+      </c>
+      <c r="C315" s="206" t="s">
+        <v>1499</v>
+      </c>
+      <c r="D315" s="213">
+        <v>44239</v>
+      </c>
+      <c r="E315" s="213">
+        <v>44243</v>
+      </c>
+      <c r="F315" s="214" t="s">
+        <v>59</v>
+      </c>
+      <c r="G315" s="214" t="s">
+        <v>1892</v>
+      </c>
+      <c r="H315" s="216" t="s">
+        <v>1893</v>
+      </c>
+      <c r="I315" s="154" t="s">
+        <v>1891</v>
+      </c>
+      <c r="K315" s="206" t="s">
+        <v>91</v>
+      </c>
+      <c r="L315" s="206" t="s">
+        <v>19</v>
+      </c>
+      <c r="M315" s="189" t="s">
+        <v>1847</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:M305" xr:uid="{2E928349-A5AA-9B41-9E5A-C956A9EBD262}">
+  <autoFilter ref="A1:M315" xr:uid="{2E928349-A5AA-9B41-9E5A-C956A9EBD262}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Que."/>
+        <filter val="N.B."/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>